<commit_message>
PDF generation with reportlab
</commit_message>
<xml_diff>
--- a/ProductReference.xlsx
+++ b/ProductReference.xlsx
@@ -690,7 +690,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -698,7 +698,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -706,7 +706,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -714,7 +714,7 @@
         <v>25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
@@ -722,7 +722,7 @@
         <v>27</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
@@ -730,7 +730,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
@@ -738,7 +738,7 @@
         <v>31</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
@@ -746,7 +746,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A18" s="2" t="s">
         <v>34</v>
       </c>
@@ -754,7 +754,7 @@
         <v>35</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A19" s="2" t="s">
         <v>36</v>
       </c>
@@ -762,7 +762,7 @@
         <v>37</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A20" s="2" t="s">
         <v>38</v>
       </c>
@@ -770,7 +770,7 @@
         <v>39</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
@@ -778,7 +778,7 @@
         <v>41</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A22" s="2" t="s">
         <v>42</v>
       </c>
@@ -786,7 +786,7 @@
         <v>43</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A23" s="2" t="s">
         <v>44</v>
       </c>
@@ -794,7 +794,7 @@
         <v>45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="3" t="s">
         <v>46</v>
       </c>
@@ -802,7 +802,7 @@
         <v>47</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="3" t="s">
         <v>48</v>
       </c>
@@ -810,7 +810,7 @@
         <v>49</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="3" t="s">
         <v>50</v>
       </c>

</xml_diff>

<commit_message>
EndUsersOrderGeneration to create pdf for table
</commit_message>
<xml_diff>
--- a/ProductReference.xlsx
+++ b/ProductReference.xlsx
@@ -818,7 +818,7 @@
         <v>51</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="3" t="s">
         <v>52</v>
       </c>
@@ -826,7 +826,7 @@
         <v>53</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="3" t="s">
         <v>54</v>
       </c>
@@ -834,7 +834,7 @@
         <v>55</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="3" t="s">
         <v>56</v>
       </c>
@@ -842,7 +842,7 @@
         <v>57</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="3" t="s">
         <v>58</v>
       </c>
@@ -850,7 +850,7 @@
         <v>59</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="3" t="s">
         <v>60</v>
       </c>
@@ -858,7 +858,7 @@
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="3" t="s">
         <v>62</v>
       </c>
@@ -866,7 +866,7 @@
         <v>63</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="3" t="s">
         <v>64</v>
       </c>
@@ -874,7 +874,7 @@
         <v>65</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="3" t="s">
         <v>66</v>
       </c>
@@ -882,7 +882,7 @@
         <v>67</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
       <c r="A35" s="3" t="s">
         <v>68</v>
       </c>

</xml_diff>